<commit_message>
Internal revision 2.0 Populated file share permissions.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C35716
</commit_message>
<xml_diff>
--- a/Project Management/eCoaching_Log_Permissions.xlsx
+++ b/Project Management/eCoaching_Log_Permissions.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14232"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14232" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions History" sheetId="2" r:id="rId1"/>
     <sheet name="Database Access" sheetId="1" r:id="rId2"/>
     <sheet name="File Share Access" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'File Share Access'!$A$1:$I$34</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
   <si>
     <t>name</t>
   </si>
@@ -151,27 +154,18 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>\\vrivscors01\BCC Scorecards\Coaching</t>
-  </si>
-  <si>
     <t>ETS</t>
   </si>
   <si>
     <t>HRInfo</t>
   </si>
   <si>
-    <t>Inactivations</t>
-  </si>
-  <si>
     <t>Outliers</t>
   </si>
   <si>
     <t>Quality</t>
   </si>
   <si>
-    <t>SDR</t>
-  </si>
-  <si>
     <t>Training</t>
   </si>
   <si>
@@ -191,13 +185,106 @@
   </si>
   <si>
     <t>AD\Virginia.Collins</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Populated Fileshare permissions</t>
+  </si>
+  <si>
+    <t>EmpInfo</t>
+  </si>
+  <si>
+    <t>Melissa Speegle</t>
+  </si>
+  <si>
+    <t>Kevin Jaquay</t>
+  </si>
+  <si>
+    <t>Scott Potter E</t>
+  </si>
+  <si>
+    <t>Jennifer Foster</t>
+  </si>
+  <si>
+    <t>Deanna Morris-Stringer</t>
+  </si>
+  <si>
+    <t>Tyler McQuillan</t>
+  </si>
+  <si>
+    <t>Jeffery Ross</t>
+  </si>
+  <si>
+    <t>Christopher Gary</t>
+  </si>
+  <si>
+    <t>John Nelson</t>
+  </si>
+  <si>
+    <t>Daniel Callahan</t>
+  </si>
+  <si>
+    <t>Jacqueline McCutcheon</t>
+  </si>
+  <si>
+    <t>Mandy Pratt</t>
+  </si>
+  <si>
+    <t>\\vrivscors01\BCC Scorecards\Coaching\</t>
+  </si>
+  <si>
+    <t>David Hinman</t>
+  </si>
+  <si>
+    <t>Doug Stearns</t>
+  </si>
+  <si>
+    <t>Lili Huang</t>
+  </si>
+  <si>
+    <t>Lisa Stein</t>
+  </si>
+  <si>
+    <t>Alison Yares</t>
+  </si>
+  <si>
+    <t>Brenda Holten</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>John Tiongson</t>
+  </si>
+  <si>
+    <t>VNGT\aspectuser (account that sends aspect files)</t>
+  </si>
+  <si>
+    <t>VNGT\QMTasks (account that sends IQS files)</t>
+  </si>
+  <si>
+    <t>SVC-F1220-PSFT (account that sends PeopleSoft file)</t>
+  </si>
+  <si>
+    <t>VNGT\sqlsscord01 (sql service account for dev instance)</t>
+  </si>
+  <si>
+    <t>VNGT\sqlsscort01 (sql service account for test instance)</t>
+  </si>
+  <si>
+    <t>VNGT\sqlsscorp01 (sql service account for prod instance)</t>
+  </si>
+  <si>
+    <t>Apps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +306,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,8 +328,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -242,11 +361,186 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -256,9 +550,52 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,13 +874,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="27.5546875" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
@@ -574,6 +913,20 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>42660</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -782,7 +1135,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -790,7 +1143,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
@@ -875,69 +1228,594 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="4" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="48.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="44"/>
+      <c r="C3" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="37"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B19" s="48"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="40"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="39" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
+      <c r="B20" s="48"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="40"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="48"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="40"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="48"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="40"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="48"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I23" s="40"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="48"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="40"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="48"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="40"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="48"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="40"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="48"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="40"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="48"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I28" s="40"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="48"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="40"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="48"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="40"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="48"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="40"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="48"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="48"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="49"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="43" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I34"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>